<commit_message>
Lecture-5 Implementing Reporting Framework
</commit_message>
<xml_diff>
--- a/src/test/java/testData/loginData.xlsx
+++ b/src/test/java/testData/loginData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OfficialStuff\10Pearls\POC\appiumDemo\src\test\java\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4717F0A8-5656-42EE-A1B0-C092BFCC7B95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18ABDEA9-C87B-4C59-90B7-431EFBD87C0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,10 +28,10 @@
     <t>password</t>
   </si>
   <si>
-    <t>Thunder27$</t>
+    <t>@mailinator.com</t>
   </si>
   <si>
-    <t>@mailinator.com</t>
+    <t>Thunder27$</t>
   </si>
 </sst>
 </file>
@@ -387,7 +387,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A8"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -406,10 +406,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>